<commit_message>
added scoring logic and whole lotta things
</commit_message>
<xml_diff>
--- a/files/Tasks.xlsx
+++ b/files/Tasks.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shahaliyev_\Desktop\Code\task-report\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shahaliyev_\Desktop\Code\task-analyzer\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE736DD6-AA0A-4547-A721-6EED5A358864}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B19DC6F-9F64-445E-9ADE-77583463F61B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="47">
   <si>
     <t>Title</t>
   </si>
@@ -88,9 +88,6 @@
     <t>Medium</t>
   </si>
   <si>
-    <t>Code python project report project</t>
-  </si>
-  <si>
     <t>Coding</t>
   </si>
   <si>
@@ -152,6 +149,18 @@
   </si>
   <si>
     <t>Translate Mammadguluzada Buz</t>
+  </si>
+  <si>
+    <t>Create VOEN account</t>
+  </si>
+  <si>
+    <t>Launch portfolio website</t>
+  </si>
+  <si>
+    <t>Completed</t>
+  </si>
+  <si>
+    <t>Code task analyzer app</t>
   </si>
 </sst>
 </file>
@@ -475,7 +484,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:J40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H6" sqref="H6"/>
@@ -483,12 +492,12 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.21875" customWidth="1"/>
+    <col min="1" max="1" width="31.5546875" customWidth="1"/>
     <col min="8" max="8" width="15.77734375" customWidth="1"/>
     <col min="9" max="9" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -520,7 +529,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
@@ -545,8 +554,9 @@
       <c r="H2" s="4">
         <v>44835</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I2" s="4"/>
+    </row>
+    <row r="3" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>14</v>
       </c>
@@ -571,8 +581,9 @@
       <c r="H3" s="4">
         <v>44805</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I3" s="4"/>
+    </row>
+    <row r="4" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>17</v>
       </c>
@@ -595,10 +606,11 @@
         <v>19</v>
       </c>
       <c r="H4" s="4">
-        <v>44927</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+        <v>45047</v>
+      </c>
+      <c r="I4" s="4"/>
+    </row>
+    <row r="5" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
@@ -621,15 +633,16 @@
         <v>19</v>
       </c>
       <c r="H5" s="4">
-        <v>44783</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+        <v>44784</v>
+      </c>
+      <c r="I5" s="4"/>
+    </row>
+    <row r="6" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>23</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>16</v>
@@ -647,15 +660,16 @@
         <v>13</v>
       </c>
       <c r="H6" s="4">
-        <v>44786</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+        <v>44790</v>
+      </c>
+      <c r="I6" s="4"/>
+    </row>
+    <row r="7" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>25</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>12</v>
@@ -675,10 +689,11 @@
       <c r="H7" s="4">
         <v>44793</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I7" s="4"/>
+    </row>
+    <row r="8" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>15</v>
@@ -701,13 +716,14 @@
       <c r="H8" s="4">
         <v>44927</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I8" s="4"/>
+    </row>
+    <row r="9" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>28</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>21</v>
@@ -727,13 +743,14 @@
       <c r="H9" s="4">
         <v>44805</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I9" s="4"/>
+    </row>
+    <row r="10" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>16</v>
@@ -753,13 +770,14 @@
       <c r="H10" s="4">
         <v>44896</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I10" s="4"/>
+    </row>
+    <row r="11" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>21</v>
@@ -779,13 +797,14 @@
       <c r="H11" s="4">
         <v>44805</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I11" s="4"/>
+    </row>
+    <row r="12" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>21</v>
@@ -805,13 +824,14 @@
       <c r="H12" s="4">
         <v>44805</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I12" s="4"/>
+    </row>
+    <row r="13" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>16</v>
@@ -831,13 +851,14 @@
       <c r="H13" s="4">
         <v>44896</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I13" s="4"/>
+    </row>
+    <row r="14" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>34</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>21</v>
@@ -857,13 +878,14 @@
       <c r="H14" s="4">
         <v>44805</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I14" s="4"/>
+    </row>
+    <row r="15" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>16</v>
@@ -883,13 +905,14 @@
       <c r="H15" s="4">
         <v>44835</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I15" s="4"/>
+    </row>
+    <row r="16" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>36</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>37</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>21</v>
@@ -909,10 +932,11 @@
       <c r="H16" s="4">
         <v>45292</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I16" s="4"/>
+    </row>
+    <row r="17" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>18</v>
@@ -935,10 +959,11 @@
       <c r="H17" s="4">
         <v>44805</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I17" s="4"/>
+    </row>
+    <row r="18" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>18</v>
@@ -961,13 +986,14 @@
       <c r="H18" s="4">
         <v>44835</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I18" s="4"/>
+    </row>
+    <row r="19" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>40</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>41</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>16</v>
@@ -987,13 +1013,14 @@
       <c r="H19" s="4">
         <v>44835</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I19" s="4"/>
+    </row>
+    <row r="20" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>21</v>
@@ -1005,7 +1032,7 @@
         <v>12</v>
       </c>
       <c r="F20" s="2">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="G20" s="2" t="s">
         <v>19</v>
@@ -1013,10 +1040,11 @@
       <c r="H20" s="4">
         <v>44927</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I20" s="4"/>
+    </row>
+    <row r="21" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>15</v>
@@ -1039,46 +1067,269 @@
       <c r="H21" s="4">
         <v>44835</v>
       </c>
+      <c r="I21" s="4"/>
+    </row>
+    <row r="22" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F22" s="2">
+        <v>4</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H22" s="4">
+        <v>44788</v>
+      </c>
+      <c r="I22" s="4"/>
+    </row>
+    <row r="23" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F23" s="2">
+        <v>40</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="H23" s="4">
+        <v>44621</v>
+      </c>
+      <c r="I23" s="4">
+        <v>44666</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="4"/>
+      <c r="I24" s="4"/>
+    </row>
+    <row r="25" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="4"/>
+    </row>
+    <row r="26" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="4"/>
+      <c r="I26" s="4"/>
+    </row>
+    <row r="27" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="4"/>
+      <c r="I27" s="4"/>
+    </row>
+    <row r="28" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="4"/>
+      <c r="I28" s="4"/>
+    </row>
+    <row r="29" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="4"/>
+      <c r="I29" s="4"/>
+    </row>
+    <row r="30" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="4"/>
+      <c r="I30" s="4"/>
+    </row>
+    <row r="31" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="4"/>
+      <c r="I31" s="4"/>
+    </row>
+    <row r="32" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
+      <c r="H32" s="4"/>
+      <c r="I32" s="4"/>
+    </row>
+    <row r="33" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="4"/>
+      <c r="I33" s="4"/>
+    </row>
+    <row r="34" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2"/>
+      <c r="H34" s="4"/>
+      <c r="I34" s="4"/>
+    </row>
+    <row r="35" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
+      <c r="H35" s="4"/>
+      <c r="I35" s="4"/>
+    </row>
+    <row r="36" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="2"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="4"/>
+      <c r="I36" s="4"/>
+    </row>
+    <row r="37" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="4"/>
+    </row>
+    <row r="38" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="2"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="4"/>
+    </row>
+    <row r="39" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="2"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2"/>
+      <c r="G39" s="2"/>
+      <c r="H39" s="4"/>
+    </row>
+    <row r="40" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="2"/>
+      <c r="C40" s="2"/>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+      <c r="F40" s="2"/>
+      <c r="G40" s="2"/>
+      <c r="H40" s="4"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="G2:G21">
+  <conditionalFormatting sqref="G2:G40">
     <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
       <formula>"Not Started"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G21">
+  <conditionalFormatting sqref="G2:G40">
     <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
       <formula>"Ongoing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G21">
+  <conditionalFormatting sqref="G2:G40">
     <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:E21">
+  <conditionalFormatting sqref="C2:E40">
     <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
       <formula>"High"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:E21">
+  <conditionalFormatting sqref="C2:E40">
     <cfRule type="cellIs" dxfId="1" priority="5" operator="equal">
       <formula>"Medium"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:E21">
+  <conditionalFormatting sqref="C2:E40">
     <cfRule type="cellIs" dxfId="0" priority="6" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" sqref="C2:E21" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" sqref="C2:E40" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"High,Medium,Low"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="G2:G21" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" sqref="G2:G40" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"Not Started,Ongoing,Completed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="B2:B21" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" sqref="B2:B40" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"Health,Family,Reading,Startup,Writing,Coding,Career,Chess,Skillset,Other"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
added create_df, sort, and other important functions
</commit_message>
<xml_diff>
--- a/files/Tasks.xlsx
+++ b/files/Tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shahaliyev_\Desktop\Code\task-analyzer\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B19DC6F-9F64-445E-9ADE-77583463F61B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3287852-4B98-4C86-8A5C-89E4F83126B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="49">
   <si>
     <t>Title</t>
   </si>
@@ -161,6 +161,12 @@
   </si>
   <si>
     <t>Code task analyzer app</t>
+  </si>
+  <si>
+    <t>Invitation mails for shusha chess</t>
+  </si>
+  <si>
+    <t>Shusha</t>
   </si>
 </sst>
 </file>
@@ -487,7 +493,7 @@
   <dimension ref="A1:J40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1126,13 +1132,30 @@
       </c>
     </row>
     <row r="24" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="4"/>
+      <c r="A24" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F24" s="2">
+        <v>2</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H24" s="4">
+        <v>44789</v>
+      </c>
       <c r="I24" s="4"/>
     </row>
     <row r="25" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added cmd line argument
</commit_message>
<xml_diff>
--- a/files/Tasks.xlsx
+++ b/files/Tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shahaliyev_\Desktop\Code\task-analyzer\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3287852-4B98-4C86-8A5C-89E4F83126B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE4BC43C-83B0-4827-A2B0-3C7F3F550BA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="37">
   <si>
     <t>Title</t>
   </si>
@@ -46,12 +46,6 @@
     <t>Deadline</t>
   </si>
   <si>
-    <t>Completion date</t>
-  </si>
-  <si>
-    <t>Notes</t>
-  </si>
-  <si>
     <t>Create teaching methodology</t>
   </si>
   <si>
@@ -64,27 +58,18 @@
     <t>Ongoing</t>
   </si>
   <si>
-    <t>Copywrite Grand Memoir</t>
-  </si>
-  <si>
     <t>Writing</t>
   </si>
   <si>
     <t>Low</t>
   </si>
   <si>
-    <t>Publish Grand Memoir</t>
-  </si>
-  <si>
     <t>Family</t>
   </si>
   <si>
     <t>Not Started</t>
   </si>
   <si>
-    <t>Create Kramnik's lecture pgn</t>
-  </si>
-  <si>
     <t>Medium</t>
   </si>
   <si>
@@ -100,9 +85,6 @@
     <t>Publish Lincoln essay</t>
   </si>
   <si>
-    <t>Read Rhetoric</t>
-  </si>
-  <si>
     <t>Reading</t>
   </si>
   <si>
@@ -115,30 +97,18 @@
     <t>Read Stendhal</t>
   </si>
   <si>
-    <t>Read Seneca</t>
-  </si>
-  <si>
     <t>Buy clothes</t>
   </si>
   <si>
     <t>Other</t>
   </si>
   <si>
-    <t>Start boxing</t>
-  </si>
-  <si>
     <t>Become Grandmaster</t>
   </si>
   <si>
     <t>Chess</t>
   </si>
   <si>
-    <t>Launch website for mother</t>
-  </si>
-  <si>
-    <t>Start bina factory</t>
-  </si>
-  <si>
     <t>Launch Youtube channel</t>
   </si>
   <si>
@@ -148,9 +118,6 @@
     <t>Become fluent in russian</t>
   </si>
   <si>
-    <t>Translate Mammadguluzada Buz</t>
-  </si>
-  <si>
     <t>Create VOEN account</t>
   </si>
   <si>
@@ -163,10 +130,7 @@
     <t>Code task analyzer app</t>
   </si>
   <si>
-    <t>Invitation mails for shusha chess</t>
-  </si>
-  <si>
-    <t>Shusha</t>
+    <t>Help a family member</t>
   </si>
 </sst>
 </file>
@@ -490,10 +454,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:J40"/>
+  <dimension ref="A1:J31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -528,34 +492,30 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
     </row>
     <row r="2" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F2" s="2">
         <v>100</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="H2" s="4">
         <v>44835</v>
@@ -564,55 +524,55 @@
     </row>
     <row r="3" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>16</v>
       </c>
       <c r="F3" s="2">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="H3" s="4">
-        <v>44805</v>
+        <v>44790</v>
       </c>
       <c r="I3" s="4"/>
     </row>
     <row r="4" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="F4" s="2">
-        <v>200</v>
+        <v>6</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="H4" s="4">
-        <v>45047</v>
+        <v>44793</v>
       </c>
       <c r="I4" s="4"/>
     </row>
@@ -621,52 +581,52 @@
         <v>20</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="2">
+        <v>100</v>
+      </c>
+      <c r="G5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F5" s="2">
-        <v>3</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>19</v>
-      </c>
       <c r="H5" s="4">
-        <v>44784</v>
+        <v>44927</v>
       </c>
       <c r="I5" s="4"/>
     </row>
     <row r="6" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="F6" s="2">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="H6" s="4">
-        <v>44790</v>
+        <v>44896</v>
       </c>
       <c r="I6" s="4"/>
     </row>
@@ -675,76 +635,76 @@
         <v>23</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="F7" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="H7" s="4">
-        <v>44793</v>
+        <v>44805</v>
       </c>
       <c r="I7" s="4"/>
     </row>
     <row r="8" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="2">
         <v>15</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8" s="2">
-        <v>100</v>
-      </c>
       <c r="G8" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="H8" s="4">
-        <v>44927</v>
+        <v>44805</v>
       </c>
       <c r="I8" s="4"/>
     </row>
     <row r="9" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="C9" s="2" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>16</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="F9" s="2">
         <v>10</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="H9" s="4">
         <v>44805</v>
@@ -753,28 +713,28 @@
     </row>
     <row r="10" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="C10" s="2" t="s">
         <v>16</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="F10" s="2">
-        <v>50</v>
+        <v>1000</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="H10" s="4">
-        <v>44896</v>
+        <v>45292</v>
       </c>
       <c r="I10" s="4"/>
     </row>
@@ -783,382 +743,227 @@
         <v>29</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="F11" s="2">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="H11" s="4">
-        <v>44805</v>
+        <v>44835</v>
       </c>
       <c r="I11" s="4"/>
     </row>
     <row r="12" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="C12" s="2" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="F12" s="2">
+        <v>500</v>
+      </c>
+      <c r="G12" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="H12" s="4">
+        <v>44927</v>
+      </c>
+      <c r="I12" s="4"/>
+    </row>
+    <row r="13" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H12" s="4">
-        <v>44805</v>
-      </c>
-      <c r="I12" s="4"/>
-    </row>
-    <row r="13" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>16</v>
-      </c>
       <c r="F13" s="2">
+        <v>4</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H13" s="4">
+        <v>44788</v>
+      </c>
+      <c r="I13" s="4"/>
+    </row>
+    <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" s="2">
         <v>40</v>
       </c>
-      <c r="G13" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H13" s="4">
-        <v>44896</v>
-      </c>
-      <c r="I13" s="4"/>
-    </row>
-    <row r="14" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F14" s="2">
-        <v>10</v>
-      </c>
       <c r="G14" s="2" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="H14" s="4">
-        <v>44805</v>
+        <v>44621</v>
       </c>
       <c r="I14" s="4"/>
     </row>
-    <row r="15" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>16</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="F15" s="2">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="H15" s="4">
-        <v>44835</v>
+        <v>44814</v>
       </c>
       <c r="I15" s="4"/>
     </row>
-    <row r="16" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F16" s="2">
-        <v>1000</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H16" s="4">
-        <v>45292</v>
-      </c>
+    <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="4"/>
       <c r="I16" s="4"/>
     </row>
-    <row r="17" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F17" s="2">
-        <v>30</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H17" s="4">
-        <v>44805</v>
-      </c>
+    <row r="17" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="4"/>
       <c r="I17" s="4"/>
     </row>
-    <row r="18" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F18" s="2">
-        <v>300</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H18" s="4">
-        <v>44835</v>
-      </c>
+    <row r="18" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="4"/>
       <c r="I18" s="4"/>
     </row>
-    <row r="19" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F19" s="2">
-        <v>30</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H19" s="4">
-        <v>44835</v>
-      </c>
+    <row r="19" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="4"/>
       <c r="I19" s="4"/>
     </row>
-    <row r="20" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F20" s="2">
-        <v>500</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H20" s="4">
-        <v>44927</v>
-      </c>
+    <row r="20" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="4"/>
       <c r="I20" s="4"/>
     </row>
-    <row r="21" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F21" s="2">
-        <v>20</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H21" s="4">
-        <v>44835</v>
-      </c>
+    <row r="21" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="4"/>
       <c r="I21" s="4"/>
     </row>
-    <row r="22" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F22" s="2">
-        <v>4</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H22" s="4">
-        <v>44788</v>
-      </c>
+    <row r="22" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="4"/>
       <c r="I22" s="4"/>
     </row>
-    <row r="23" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F23" s="2">
-        <v>40</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="H23" s="4">
-        <v>44621</v>
-      </c>
-      <c r="I23" s="4">
-        <v>44666</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F24" s="2">
-        <v>2</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H24" s="4">
-        <v>44789</v>
-      </c>
+    <row r="23" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="4"/>
+      <c r="I23" s="4"/>
+    </row>
+    <row r="24" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="4"/>
       <c r="I24" s="4"/>
     </row>
-    <row r="25" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
@@ -1168,7 +973,7 @@
       <c r="H25" s="4"/>
       <c r="I25" s="4"/>
     </row>
-    <row r="26" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
@@ -1178,7 +983,7 @@
       <c r="H26" s="4"/>
       <c r="I26" s="4"/>
     </row>
-    <row r="27" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
@@ -1188,7 +993,7 @@
       <c r="H27" s="4"/>
       <c r="I27" s="4"/>
     </row>
-    <row r="28" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
@@ -1196,9 +1001,8 @@
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
       <c r="H28" s="4"/>
-      <c r="I28" s="4"/>
-    </row>
-    <row r="29" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
@@ -1206,9 +1010,8 @@
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
       <c r="H29" s="4"/>
-      <c r="I29" s="4"/>
-    </row>
-    <row r="30" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
@@ -1216,9 +1019,8 @@
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
       <c r="H30" s="4"/>
-      <c r="I30" s="4"/>
-    </row>
-    <row r="31" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
@@ -1226,133 +1028,46 @@
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
       <c r="H31" s="4"/>
-      <c r="I31" s="4"/>
-    </row>
-    <row r="32" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
-      <c r="G32" s="2"/>
-      <c r="H32" s="4"/>
-      <c r="I32" s="4"/>
-    </row>
-    <row r="33" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
-      <c r="G33" s="2"/>
-      <c r="H33" s="4"/>
-      <c r="I33" s="4"/>
-    </row>
-    <row r="34" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
-      <c r="G34" s="2"/>
-      <c r="H34" s="4"/>
-      <c r="I34" s="4"/>
-    </row>
-    <row r="35" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="2"/>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
-      <c r="F35" s="2"/>
-      <c r="G35" s="2"/>
-      <c r="H35" s="4"/>
-      <c r="I35" s="4"/>
-    </row>
-    <row r="36" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="2"/>
-      <c r="C36" s="2"/>
-      <c r="D36" s="2"/>
-      <c r="E36" s="2"/>
-      <c r="F36" s="2"/>
-      <c r="G36" s="2"/>
-      <c r="H36" s="4"/>
-      <c r="I36" s="4"/>
-    </row>
-    <row r="37" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="2"/>
-      <c r="C37" s="2"/>
-      <c r="D37" s="2"/>
-      <c r="E37" s="2"/>
-      <c r="F37" s="2"/>
-      <c r="G37" s="2"/>
-      <c r="H37" s="4"/>
-    </row>
-    <row r="38" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="2"/>
-      <c r="C38" s="2"/>
-      <c r="D38" s="2"/>
-      <c r="E38" s="2"/>
-      <c r="F38" s="2"/>
-      <c r="G38" s="2"/>
-      <c r="H38" s="4"/>
-    </row>
-    <row r="39" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="2"/>
-      <c r="C39" s="2"/>
-      <c r="D39" s="2"/>
-      <c r="E39" s="2"/>
-      <c r="F39" s="2"/>
-      <c r="G39" s="2"/>
-      <c r="H39" s="4"/>
-    </row>
-    <row r="40" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="2"/>
-      <c r="C40" s="2"/>
-      <c r="D40" s="2"/>
-      <c r="E40" s="2"/>
-      <c r="F40" s="2"/>
-      <c r="G40" s="2"/>
-      <c r="H40" s="4"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="G2:G40">
+  <conditionalFormatting sqref="G2:G31">
     <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
       <formula>"Not Started"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G40">
+  <conditionalFormatting sqref="G2:G31">
     <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
       <formula>"Ongoing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G40">
+  <conditionalFormatting sqref="G2:G31">
     <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:E40">
+  <conditionalFormatting sqref="C2:E31">
     <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
       <formula>"High"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:E40">
+  <conditionalFormatting sqref="C2:E31">
     <cfRule type="cellIs" dxfId="1" priority="5" operator="equal">
       <formula>"Medium"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:E40">
+  <conditionalFormatting sqref="C2:E31">
     <cfRule type="cellIs" dxfId="0" priority="6" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" sqref="C2:E40" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" sqref="C2:E31" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"High,Medium,Low"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="G2:G40" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" sqref="G2:G31" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"Not Started,Ongoing,Completed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="B2:B40" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" sqref="B2:B31" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"Health,Family,Reading,Startup,Writing,Coding,Career,Chess,Skillset,Other"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>